<commit_message>
split i to filer
</commit_message>
<xml_diff>
--- a/ExcelFiles/SynxCat_test_sheet1.xlsx
+++ b/ExcelFiles/SynxCat_test_sheet1.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -429,7 +429,7 @@
         <v>Count</v>
       </c>
       <c r="B3" t="str">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" t="str">
         <v>Count</v>
@@ -496,10 +496,10 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>tja</v>
+        <v>timestamp</v>
       </c>
       <c r="B8" t="str">
-        <v>noen banket på døren</v>
+        <v>2023-11-23 14:40:00.000</v>
       </c>
       <c r="C8" t="str">
         <v>format</v>
@@ -510,23 +510,39 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>hallo</v>
+        <v>sentfrom</v>
       </c>
       <c r="B9" t="str">
-        <v>Går tur til stranda på Brusand</v>
+        <v>holla</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>bjeff</v>
+        <v>mottaker</v>
       </c>
       <c r="B10" t="str">
-        <v>VOFF</v>
+        <v>The Stig</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>tema</v>
+      </c>
+      <c r="B11" t="str">
+        <v>fast car ride</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>payload</v>
+      </c>
+      <c r="B12" t="str">
+        <v>{"id": 123, "name":"Per Spellmann","address":"alle de som æ ø å Æ Ø Å spelle kan de hører hjemme i spelleland", "wish":"han hadde ei einaste ku"}</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>